<commit_message>
Rrxcell::Sheet#address implemented - Rrxcell::Cell can get with A1-format address - Raise RuntimeError with invalid cell address - Rrxcell::Book#sheet_names give String Array, #sheets give Rrxcell::Sheet Array - Rrxcell::Book#sheet can get sheet with sheet-name
</commit_message>
<xml_diff>
--- a/example/book.xlsx
+++ b/example/book.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1900" windowWidth="13880" windowHeight="11460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="13380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Sheet1!A1</t>
     <phoneticPr fontId="1"/>
@@ -210,6 +210,36 @@
   </si>
   <si>
     <t>Sheet1!C20</t>
+  </si>
+  <si>
+    <t>Sheet1!AA1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sheet1!AA2</t>
+  </si>
+  <si>
+    <t>Sheet1!AA3</t>
+  </si>
+  <si>
+    <t>Sheet1!AB1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sheet1!AC1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sheet1!AB2</t>
+  </si>
+  <si>
+    <t>Sheet1!AC2</t>
+  </si>
+  <si>
+    <t>Sheet1!AB3</t>
+  </si>
+  <si>
+    <t>Sheet1!AC3</t>
   </si>
 </sst>
 </file>
@@ -533,18 +563,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,8 +592,17 @@
         <f>D1</f>
         <v>42370</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="AA1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -579,8 +619,17 @@
         <f t="shared" ref="E2:E3" si="0">D2</f>
         <v>42370.416666666664</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="AA2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -597,8 +646,17 @@
         <f t="shared" si="0"/>
         <v>0.4309027777777778</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="AA3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -609,7 +667,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -620,7 +678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -631,7 +689,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -642,7 +700,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -653,7 +711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -664,7 +722,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -675,7 +733,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -686,7 +744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -697,7 +755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -708,7 +766,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -719,7 +777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -730,7 +788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -788,5 +846,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>